<commit_message>
Added all class project deadlines; Color Code
</commit_message>
<xml_diff>
--- a/Important Dates & Deadlines.xlsx
+++ b/Important Dates & Deadlines.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Important Dates and Deadlines:</t>
   </si>
   <si>
-    <t>Last updated: 01/24/2017 4:17 PM by Carlos Castro</t>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -81,13 +78,58 @@
   </si>
   <si>
     <t>Available until 2/8; Must meet prior to pick a topic</t>
+  </si>
+  <si>
+    <t>Update Divide and Conquer Files</t>
+  </si>
+  <si>
+    <t>Assignment opens 2/13</t>
+  </si>
+  <si>
+    <t>due via webcourses</t>
+  </si>
+  <si>
+    <t>Table of Contents Submission</t>
+  </si>
+  <si>
+    <t>Table of Contents, Due via webcourses</t>
+  </si>
+  <si>
+    <t>Current Draft of Senior Design 1 Documentation</t>
+  </si>
+  <si>
+    <t>30 - 60% of paper should be complete</t>
+  </si>
+  <si>
+    <t>Meet with Dr. Wei after to discuss Table of Contents and Draft</t>
+  </si>
+  <si>
+    <t>Assignment opens 04/10</t>
+  </si>
+  <si>
+    <t>Final Document Due</t>
+  </si>
+  <si>
+    <t>Last updated: 01/24/2017 6:42 PM by Carlos Castro</t>
+  </si>
+  <si>
+    <t>Key:</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Meeting/Event</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,16 +153,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -128,36 +203,290 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +810,7 @@
     <col min="1" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="75.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -490,85 +819,197 @@
       </c>
       <c r="B1" s="2"/>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D6" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>42769</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>42770</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>42769</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="D8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>42774</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>42783</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>42818</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>42825</v>
+      </c>
+      <c r="B12" s="13">
         <v>0.5</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>42770</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>42774</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>42852</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="C13" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Selected 2 projects to present based on 1/26 meeting
</commit_message>
<xml_diff>
--- a/Important Dates & Deadlines.xlsx
+++ b/Important Dates & Deadlines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Important Dates and Deadlines:</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Final Document Due</t>
   </si>
   <si>
-    <t>Last updated: 01/24/2017 6:42 PM by Carlos Castro</t>
-  </si>
-  <si>
     <t>Key:</t>
   </si>
   <si>
@@ -120,6 +117,141 @@
   </si>
   <si>
     <t>Initial Document 10 pages, due via webcourses</t>
+  </si>
+  <si>
+    <t>Divide and Conquer Soft Deadline</t>
+  </si>
+  <si>
+    <r>
+      <t>Carlos:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project Milestones</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; Patrick:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project Block Diagram (maybe include prototype illustration) (work with everyone, mostly project milestones)
+  - Decision matrix (work with me, if help needed)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; Courtnie: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- House of Quality Trade Off table
+  - requirement specifications (engineering requirements) (work with 2 for goals and objectives)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; Lucas: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- budget and financing (work with 3, for requirement specifications)
+  - goals and objectives (marketing requirements)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; 
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Fire Alarm 
+Goals and Objectives
+- gives clear direction in case of emergency
+- market more toward hotels and office buildings
+- same batteries as smoke alarms
+- low power, low cost
+Engineering Requirements
+- same batteries as smoke alarms
+- Smoke sensor standard from fire departments
+- two LEDs
+- Transmitter and Receiver
+- CPU unit, very simple one
+- Battery signal or light
+- software to handle case 
+- C++ or Python</t>
+  </si>
+  <si>
+    <t>Teaching Assistant
+Goals and Objectives
+- low cost, low power
+- help kids learn easily without needing expensive tablet/phone
+- Teacher can assign for student to practice
+- keeps track of scores
+Engineering Requirements
+- LED or LCD screen
+- Microphone
+- Battery (rechargable)
+- speech recognition software
+- CPU, more advanced
+- memory to hold apps and resulting data
+- User Interface
+- Input keys
+- USB port to load in assignments
+- Portable</t>
+  </si>
+  <si>
+    <t>Last updated: 01/26/2017 8:35 PM by Carlos Castro</t>
   </si>
 </sst>
 </file>
@@ -195,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -405,6 +537,39 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -412,7 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -484,6 +649,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -799,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,39 +991,40 @@
     <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="75.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="33"/>
       <c r="C4" s="34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>1</v>
       </c>
@@ -863,141 +1044,158 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+    <row r="7" spans="1:7" s="41" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>42767</v>
+      </c>
+      <c r="B7" s="36">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
         <v>42769</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B8" s="24">
         <v>0.5</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26" t="s">
+      <c r="D8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
         <v>42770</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F9" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
         <v>42774</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B10" s="10">
         <v>0.52083333333333337</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <v>42783</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="17" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
         <v>42818</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B12" s="13">
         <v>0.99930555555555556</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="E12" s="12"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
         <v>42825</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B13" s="13">
         <v>0.5</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="17" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
         <v>42852</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B14" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22" t="s">
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
@@ -1007,9 +1205,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Deadlines and Meetings
</commit_message>
<xml_diff>
--- a/Important Dates & Deadlines.xlsx
+++ b/Important Dates & Deadlines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Important Dates and Deadlines:</t>
   </si>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>due via webcourses</t>
-  </si>
-  <si>
-    <t>Table of Contents Submission</t>
-  </si>
-  <si>
-    <t>Table of Contents, Due via webcourses</t>
   </si>
   <si>
     <t>Current Draft of Senior Design 1 Documentation</t>
@@ -251,7 +245,34 @@
 - Portable</t>
   </si>
   <si>
-    <t>Last updated: 01/26/2017 8:35 PM by Carlos Castro</t>
+    <t>Group Meeting</t>
+  </si>
+  <si>
+    <t>Updated Initial Document Files</t>
+  </si>
+  <si>
+    <t>Updated Files</t>
+  </si>
+  <si>
+    <t>Continue working on research</t>
+  </si>
+  <si>
+    <t>First Round of Assigned Research Documentation</t>
+  </si>
+  <si>
+    <t>Research Documentation</t>
+  </si>
+  <si>
+    <t>Check with Carlos for guidance</t>
+  </si>
+  <si>
+    <t>100 Page Submission</t>
+  </si>
+  <si>
+    <t>25 Pages Each due</t>
+  </si>
+  <si>
+    <t>Last updated: 02/09/2017 8:35 PM by Carlos Castro</t>
   </si>
 </sst>
 </file>
@@ -327,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -569,6 +590,45 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -577,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -664,6 +724,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -979,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -988,8 +1061,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="75.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="49.5703125" customWidth="1"/>
   </cols>
@@ -1000,27 +1074,27 @@
       </c>
       <c r="B1" s="2"/>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="33"/>
       <c r="C4" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1052,17 +1126,17 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1076,7 +1150,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="26" t="s">
@@ -1123,81 +1197,113 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>42781</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>42783</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="17" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>42818</v>
-      </c>
-      <c r="B12" s="13">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="C12" s="12" t="s">
+    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
+        <v>42788</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>42825</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>42825</v>
-      </c>
-      <c r="B13" s="13">
+      <c r="E14" s="12"/>
+      <c r="F14" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43">
+        <v>42839</v>
+      </c>
+      <c r="B15" s="44">
         <v>0.5</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+    </row>
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>42852</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
-        <v>42852</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1209,9 +1315,17 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Results of 2/15 meeting, as well as changes for "Updates" document
</commit_message>
<xml_diff>
--- a/Important Dates & Deadlines.xlsx
+++ b/Important Dates & Deadlines.xlsx
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Current Draft of Senior Design 1 Documentation</t>
-  </si>
-  <si>
-    <t>30 - 60% of paper should be complete</t>
   </si>
   <si>
     <t>Meet with Dr. Wei after to discuss Table of Contents and Draft</t>
@@ -272,7 +269,10 @@
     <t>25 Pages Each due</t>
   </si>
   <si>
-    <t>Last updated: 02/09/2017 8:35 PM by Carlos Castro</t>
+    <t>30 - 60% of paper should be complete (60 Pages)</t>
+  </si>
+  <si>
+    <t>Last updated: 02/15/2017 12:28 PM by Carlos Castro</t>
   </si>
 </sst>
 </file>
@@ -1080,21 +1080,21 @@
     <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="33"/>
       <c r="C4" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1126,17 +1126,17 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="C7" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="38" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>30</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="40" t="s">
         <v>31</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="26" t="s">
@@ -1205,16 +1205,16 @@
         <v>0.5</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1243,16 +1243,16 @@
         <v>0.5</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1266,11 +1266,11 @@
         <v>20</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1281,10 +1281,10 @@
         <v>0.5</v>
       </c>
       <c r="C15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>41</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="46"/>
@@ -1297,12 +1297,12 @@
         <v>13</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lucas initial docs (#5)
* Added narrative for fire alarms

* Teacher Tool

added the project narrative for the teacher tool

* Minor text fixes

* Added Project Timeline

* Started Compiling all of the parts, some minor changes made

* Formatting and Organizational Changes

* Add files via upload

* Updated Documentation,: Financial plan, House of Quality, Engineering Requirements

* Added in budget for Teaching Assistant

* Minor Text Fixes to Project Narrative AND First Draft

* Completed Final Draft of Initial Documentation

* Started Making Changes for Updating Initial Documentation

* Updated Deadlines and Meetings

* Project Timeline Updated Finished

* Add files via upload

* Added ease of installation

* Results of 2/15 meeting, as well as changes for "Updates" document

* Block Diagram and Updated Engineering Requirements

* Added a .gitignore file so that we can ignore files like .DS_Store
</commit_message>
<xml_diff>
--- a/Important Dates & Deadlines.xlsx
+++ b/Important Dates & Deadlines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Important Dates and Deadlines:</t>
   </si>
@@ -86,16 +86,7 @@
     <t>due via webcourses</t>
   </si>
   <si>
-    <t>Table of Contents Submission</t>
-  </si>
-  <si>
-    <t>Table of Contents, Due via webcourses</t>
-  </si>
-  <si>
     <t>Current Draft of Senior Design 1 Documentation</t>
-  </si>
-  <si>
-    <t>30 - 60% of paper should be complete</t>
   </si>
   <si>
     <t>Meet with Dr. Wei after to discuss Table of Contents and Draft</t>
@@ -251,7 +242,37 @@
 - Portable</t>
   </si>
   <si>
-    <t>Last updated: 01/26/2017 8:35 PM by Carlos Castro</t>
+    <t>Group Meeting</t>
+  </si>
+  <si>
+    <t>Updated Initial Document Files</t>
+  </si>
+  <si>
+    <t>Updated Files</t>
+  </si>
+  <si>
+    <t>Continue working on research</t>
+  </si>
+  <si>
+    <t>First Round of Assigned Research Documentation</t>
+  </si>
+  <si>
+    <t>Research Documentation</t>
+  </si>
+  <si>
+    <t>Check with Carlos for guidance</t>
+  </si>
+  <si>
+    <t>100 Page Submission</t>
+  </si>
+  <si>
+    <t>25 Pages Each due</t>
+  </si>
+  <si>
+    <t>30 - 60% of paper should be complete (60 Pages)</t>
+  </si>
+  <si>
+    <t>Last updated: 02/15/2017 12:28 PM by Carlos Castro</t>
   </si>
 </sst>
 </file>
@@ -327,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -569,6 +590,45 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -577,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -664,6 +724,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -979,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -988,8 +1061,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="75.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="49.5703125" customWidth="1"/>
   </cols>
@@ -1000,27 +1074,27 @@
       </c>
       <c r="B1" s="2"/>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="33"/>
       <c r="C4" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1052,17 +1126,17 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1076,7 +1150,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="26" t="s">
@@ -1123,81 +1197,113 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>42781</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>42783</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="17" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>42818</v>
-      </c>
-      <c r="B12" s="13">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="C12" s="12" t="s">
+    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
+        <v>42788</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>42825</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>42825</v>
-      </c>
-      <c r="B13" s="13">
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43">
+        <v>42839</v>
+      </c>
+      <c r="B15" s="44">
         <v>0.5</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+    </row>
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>42852</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
-        <v>42852</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1209,9 +1315,17 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated after meeting on 3-1-17
</commit_message>
<xml_diff>
--- a/Important Dates & Deadlines.xlsx
+++ b/Important Dates & Deadlines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Important Dates and Deadlines:</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Last updated: 02/15/2017 12:28 PM by Carlos Castro</t>
+  </si>
+  <si>
+    <t>12:00PM</t>
+  </si>
+  <si>
+    <t>Finish initial research, draw schematics, buy parts</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,77 +1261,93 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42">
+        <v>42802</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
         <v>42825</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B15" s="13">
         <v>0.5</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="17" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+    <row r="16" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="43">
         <v>42839</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B16" s="44">
         <v>0.5</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C16" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46"/>
-    </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
         <v>42852</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B17" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22" t="s">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>